<commit_message>
Update results.xlsx with KW21 and KW22 data
The results.xlsx file has been updated to include the latest data or analysis. No changes to code or logic were made.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/070ad96b16b63f9e/Documents/GitHub/Kata_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{493C2A2F-064F-423D-BBDF-517F9E9BECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C4221E-C045-44FD-AFFE-6A66DF2725A4}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{493C2A2F-064F-423D-BBDF-517F9E9BECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0E774CE-6663-4D99-AF10-5F170C6C9253}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Avg Time (s)</t>
   </si>
@@ -139,6 +139,14 @@
   </si>
   <si>
     <t>KW20-b28c512nbt-0930</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KW21-b28c512nbt-1001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KW22-b28c512nbt-1002</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -227,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -267,6 +275,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -286,11 +297,11 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -354,11 +365,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0520CD6C-6843-47E1-8F99-E28CA56DB791}" name="表1" displayName="表1" ref="A1:O13" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:O13" xr:uid="{0520CD6C-6843-47E1-8F99-E28CA56DB791}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0520CD6C-6843-47E1-8F99-E28CA56DB791}" name="表1" displayName="表1" ref="A1:O15" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:O15" xr:uid="{0520CD6C-6843-47E1-8F99-E28CA56DB791}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O13">
-    <sortCondition ref="K1:K13"/>
+    <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{7154B60C-CF6A-4D88-8F3E-007DE45BC89A}" name="Models"/>
@@ -377,17 +392,17 @@
     <tableColumn id="10" xr3:uid="{E6AC9C94-2A27-4D7D-8E75-25B5F03AAF48}" name="Calculated Elo" dataDxfId="5">
       <calculatedColumnFormula>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{69468EA2-E6AA-4317-99B0-7EE03E7F1D74}" name="Rank" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{69468EA2-E6AA-4317-99B0-7EE03E7F1D74}" name="Rank" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.RANK.EQ(J2, $J$2:$J$15, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{7A29C0B7-CF79-4CAD-8A54-F99D468FAC31}" name="Weighted Elo" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{7A29C0B7-CF79-4CAD-8A54-F99D468FAC31}" name="Weighted Elo" dataDxfId="3">
       <calculatedColumnFormula>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{5545508D-38B5-44B8-8DFA-711A05E197FD}" name="Samples" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{2200399E-ADD7-4B7A-BD06-CA49505DC8EA}" name="Elo Realistic" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{5545508D-38B5-44B8-8DFA-711A05E197FD}" name="Samples" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{2200399E-ADD7-4B7A-BD06-CA49505DC8EA}" name="Elo Realistic" dataDxfId="1">
       <calculatedColumnFormula>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{3428F20D-B756-4F5A-938E-E24559B1B202}" name="Efficiency" dataDxfId="1">
+    <tableColumn id="14" xr3:uid="{3428F20D-B756-4F5A-938E-E24559B1B202}" name="Efficiency" dataDxfId="0">
       <calculatedColumnFormula>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -688,7 +703,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -756,344 +771,344 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="D2">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>70</v>
-      </c>
-      <c r="F2">
-        <v>390.03699999999998</v>
-      </c>
-      <c r="G2" s="12">
-        <v>215506</v>
-      </c>
-      <c r="H2">
+      <c r="B2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8">
         <v>14085</v>
       </c>
-      <c r="I2">
-        <v>147.19</v>
+      <c r="I2" s="8">
+        <v>0</v>
       </c>
       <c r="J2">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14232.19</v>
+        <v>14085</v>
       </c>
       <c r="K2">
         <f>_xlfn.RANK.EQ(J2, $J$2:$J$15, 0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>14144.772574995735</v>
-      </c>
-      <c r="M2">
-        <v>3505824</v>
+        <v>11268</v>
       </c>
       <c r="N2">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4674</v>
-      </c>
-      <c r="O2">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>552.52706794483606</v>
+        <v>4660</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="8">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8">
         <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>9</v>
-      </c>
-      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="E3" s="8">
         <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>55.000000000000007</v>
-      </c>
-      <c r="F3">
-        <v>389.53</v>
-      </c>
-      <c r="G3" s="12">
-        <v>217964</v>
-      </c>
-      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="8">
+        <v>341.18200000000002</v>
+      </c>
+      <c r="G3" s="9">
+        <v>192826</v>
+      </c>
+      <c r="H3" s="8">
         <v>14085</v>
       </c>
-      <c r="I3">
-        <v>35.22</v>
+      <c r="I3" s="8">
+        <v>-155.63</v>
       </c>
       <c r="J3">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14120.22</v>
+        <v>13929.37</v>
       </c>
       <c r="K3">
         <f>_xlfn.RANK.EQ(J3, $J$2:$J$15, 0)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="L3" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>14068.314786161034</v>
+        <v>13905.603668851065</v>
       </c>
       <c r="M3">
-        <v>3050944</v>
+        <v>50000</v>
       </c>
       <c r="N3">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4663</v>
+        <v>4643</v>
       </c>
       <c r="O3">
         <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>559.55638846815395</v>
+        <v>565.17049551265893</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10">
         <v>20</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="8">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10">
         <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>10</v>
-      </c>
-      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10">
         <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>408.81299999999999</v>
-      </c>
-      <c r="G4" s="12">
-        <v>230241</v>
-      </c>
-      <c r="H4">
+        <v>45</v>
+      </c>
+      <c r="F4" s="8">
+        <v>351.03699999999998</v>
+      </c>
+      <c r="G4" s="11">
+        <v>195286</v>
+      </c>
+      <c r="H4" s="10">
         <v>14085</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="10">
+        <v>-35.22</v>
+      </c>
+      <c r="J4">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14085</v>
+        <v>14049.78</v>
       </c>
       <c r="K4">
         <f>_xlfn.RANK.EQ(J4, $J$2:$J$15, 0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L4" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>14051.200309777767</v>
+        <v>13982.13930163722</v>
       </c>
       <c r="M4">
-        <v>2840000</v>
+        <v>200000</v>
       </c>
       <c r="N4">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4660</v>
+        <v>4656</v>
       </c>
       <c r="O4">
         <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>563.19392974293874</v>
+        <v>556.31172782356282</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="8">
+        <v>14</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>8</v>
+      </c>
+      <c r="D5" s="10">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="10">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>40</v>
+      </c>
+      <c r="F5" s="10">
+        <v>369.678</v>
+      </c>
+      <c r="G5" s="9">
+        <v>207036</v>
+      </c>
+      <c r="H5" s="10">
         <v>14085</v>
       </c>
-      <c r="I5" s="8">
-        <v>0</v>
+      <c r="I5" s="10">
+        <v>-70.44</v>
       </c>
       <c r="J5">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14085</v>
+        <v>14014.56</v>
       </c>
       <c r="K5">
         <f>_xlfn.RANK.EQ(J5, $J$2:$J$15, 0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L5" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>11268</v>
+        <v>13965.441542534387</v>
+      </c>
+      <c r="M5">
+        <v>400000</v>
       </c>
       <c r="N5">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4660</v>
+        <v>4652</v>
+      </c>
+      <c r="O5">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>560.04414652751859</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>369.541</v>
+      </c>
+      <c r="G6" s="12">
+        <v>210117</v>
+      </c>
+      <c r="H6">
+        <v>14085</v>
+      </c>
+      <c r="I6">
+        <v>-226.07</v>
+      </c>
+      <c r="J6">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>13858.93</v>
+      </c>
+      <c r="K6">
+        <f>_xlfn.RANK.EQ(J6, $J$2:$J$15, 0)</f>
+        <v>14</v>
+      </c>
+      <c r="L6" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>13851.907010531004</v>
+      </c>
+      <c r="M6">
+        <v>600000</v>
+      </c>
+      <c r="N6">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4635</v>
+      </c>
+      <c r="O6">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>568.58914166493025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
         <v>13</v>
       </c>
-      <c r="B6" s="10">
+      <c r="E7">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>361.964</v>
+      </c>
+      <c r="G7" s="9">
+        <v>202978</v>
+      </c>
+      <c r="H7">
+        <v>14085</v>
+      </c>
+      <c r="I7">
+        <v>-120.41</v>
+      </c>
+      <c r="J7">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>13964.59</v>
+      </c>
+      <c r="K7">
+        <f>_xlfn.RANK.EQ(J7, $J$2:$J$15, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="L7" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>13919.19557133775</v>
+      </c>
+      <c r="M7">
+        <v>1240000</v>
+      </c>
+      <c r="N7">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4647</v>
+      </c>
+      <c r="O7">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>560.76847421290518</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>20</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C8">
         <v>9</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D8">
         <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
         <v>11</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E8">
         <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
         <v>45</v>
       </c>
-      <c r="F6" s="8">
-        <v>351.03699999999998</v>
-      </c>
-      <c r="G6" s="11">
-        <v>195286</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="F8">
+        <v>333.46499999999997</v>
+      </c>
+      <c r="G8" s="12">
+        <v>186586</v>
+      </c>
+      <c r="H8">
         <v>14085</v>
       </c>
-      <c r="I6" s="10">
-        <v>-35.22</v>
-      </c>
-      <c r="J6">
-        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14049.78</v>
-      </c>
-      <c r="K6">
-        <f>_xlfn.RANK.EQ(J6, $J$2:$J$15, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="L6" s="16">
-        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13982.13930163722</v>
-      </c>
-      <c r="M6">
-        <v>200000</v>
-      </c>
-      <c r="N6">
-        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4656</v>
-      </c>
-      <c r="O6">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>556.31172782356282</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>45</v>
-      </c>
-      <c r="F7">
-        <v>333.46499999999997</v>
-      </c>
-      <c r="G7" s="12">
-        <v>186586</v>
-      </c>
-      <c r="H7">
-        <v>14085</v>
-      </c>
-      <c r="I7">
+      <c r="I8">
         <v>-38.380000000000003</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
         <v>14046.62</v>
-      </c>
-      <c r="K7">
-        <f>_xlfn.RANK.EQ(J7, $J$2:$J$15, 0)</f>
-        <v>6</v>
-      </c>
-      <c r="L7" s="16">
-        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13994.889698575931</v>
-      </c>
-      <c r="M7">
-        <v>1940000</v>
-      </c>
-      <c r="N7">
-        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4656</v>
-      </c>
-      <c r="O7">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>559.53698289175782</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="10">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10">
-        <v>8</v>
-      </c>
-      <c r="D8" s="10">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>12</v>
-      </c>
-      <c r="E8" s="10">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>40</v>
-      </c>
-      <c r="F8" s="10">
-        <v>369.678</v>
-      </c>
-      <c r="G8" s="9">
-        <v>207036</v>
-      </c>
-      <c r="H8" s="10">
-        <v>14085</v>
-      </c>
-      <c r="I8" s="10">
-        <v>-70.44</v>
-      </c>
-      <c r="J8">
-        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>14014.56</v>
       </c>
       <c r="K8">
         <f>_xlfn.RANK.EQ(J8, $J$2:$J$15, 0)</f>
@@ -1101,293 +1116,397 @@
       </c>
       <c r="L8" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13965.441542534387</v>
+        <v>13994.889698575931</v>
       </c>
       <c r="M8">
-        <v>400000</v>
+        <v>1940000</v>
       </c>
       <c r="N8">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4652</v>
+        <v>4656</v>
       </c>
       <c r="O8">
         <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>560.04414652751859</v>
+        <v>559.53698289175782</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <v>364.02600000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>207507</v>
+      </c>
+      <c r="H9" s="1">
+        <v>14085</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-155.63</v>
+      </c>
+      <c r="J9">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>13929.37</v>
+      </c>
+      <c r="K9">
+        <f>_xlfn.RANK.EQ(J9, $J$2:$J$15, 0)</f>
+        <v>12</v>
+      </c>
+      <c r="L9" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>13929.37</v>
+      </c>
+      <c r="M9">
+        <v>2640000</v>
+      </c>
+      <c r="N9">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4643</v>
+      </c>
+      <c r="O9">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>570.0334591485223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>408.81299999999999</v>
+      </c>
+      <c r="G10" s="12">
+        <v>230241</v>
+      </c>
+      <c r="H10">
+        <v>14085</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>14085</v>
+      </c>
+      <c r="K10">
+        <f>_xlfn.RANK.EQ(J10, $J$2:$J$15, 0)</f>
+        <v>4</v>
+      </c>
+      <c r="L10" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>14051.200309777767</v>
+      </c>
+      <c r="M10">
+        <v>2840000</v>
+      </c>
+      <c r="N10">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4660</v>
+      </c>
+      <c r="O10">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>563.19392974293874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="F11">
+        <v>389.53</v>
+      </c>
+      <c r="G11" s="12">
+        <v>217964</v>
+      </c>
+      <c r="H11">
+        <v>14085</v>
+      </c>
+      <c r="I11">
+        <v>35.22</v>
+      </c>
+      <c r="J11">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>14120.22</v>
+      </c>
+      <c r="K11">
+        <f>_xlfn.RANK.EQ(J11, $J$2:$J$15, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="L11" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>14068.314786161034</v>
+      </c>
+      <c r="M11">
+        <v>3050944</v>
+      </c>
+      <c r="N11">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4663</v>
+      </c>
+      <c r="O11">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>559.55638846815395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>70</v>
+      </c>
+      <c r="F12">
+        <v>390.03699999999998</v>
+      </c>
+      <c r="G12" s="12">
+        <v>215506</v>
+      </c>
+      <c r="H12">
+        <v>14085</v>
+      </c>
+      <c r="I12">
+        <v>147.19</v>
+      </c>
+      <c r="J12">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>14232.19</v>
+      </c>
+      <c r="K12">
+        <f>_xlfn.RANK.EQ(J12, $J$2:$J$15, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>14144.772574995735</v>
+      </c>
+      <c r="M12">
+        <v>3505824</v>
+      </c>
+      <c r="N12">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4674</v>
+      </c>
+      <c r="O12">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>552.52706794483606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B13">
         <v>20</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C13">
         <v>8</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D13">
         <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
         <v>12</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E13">
         <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
         <v>40</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F13">
         <v>414.536</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G13" s="12">
         <v>234525</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H13">
         <v>14085</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I13">
         <v>-70.44</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J13">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
         <v>14014.56</v>
       </c>
-      <c r="K9" s="18">
-        <f>_xlfn.RANK.EQ(J9, $J$2:$J$15, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="L9" s="19">
+      <c r="K13">
+        <f>_xlfn.RANK.EQ(J13, $J$2:$J$15, 0)</f>
+        <v>8</v>
+      </c>
+      <c r="L13" s="16">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
         <v>13993.512721444835</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M13">
         <v>3525824</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N13">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
         <v>4652</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O13">
         <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
         <v>565.7530347183357</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="17">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="C14" s="17">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="D14" s="18">
         <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
         <v>13</v>
       </c>
-      <c r="E10">
+      <c r="E14" s="18">
         <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
         <v>35</v>
       </c>
-      <c r="F10">
-        <v>361.964</v>
-      </c>
-      <c r="G10" s="9">
-        <v>202978</v>
-      </c>
-      <c r="H10">
+      <c r="F14" s="17">
+        <v>391.483</v>
+      </c>
+      <c r="G14" s="20">
+        <v>219283</v>
+      </c>
+      <c r="H14" s="17">
         <v>14085</v>
       </c>
-      <c r="I10">
+      <c r="I14" s="17">
         <v>-120.41</v>
       </c>
-      <c r="J10">
+      <c r="J14" s="18">
         <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
         <v>13964.59</v>
       </c>
-      <c r="K10">
-        <f>_xlfn.RANK.EQ(J10, $J$2:$J$15, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="L10" s="16">
+      <c r="K14" s="18">
+        <f>_xlfn.RANK.EQ(J14, $J$2:$J$15, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="L14" s="19">
         <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13919.19557133775</v>
-      </c>
-      <c r="M10">
-        <v>1240000</v>
-      </c>
-      <c r="N10">
+        <v>13916.087688367335</v>
+      </c>
+      <c r="M14" s="18">
+        <v>3600000</v>
+      </c>
+      <c r="N14" s="18">
         <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
         <v>4647</v>
       </c>
-      <c r="O10">
+      <c r="O14" s="18">
         <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>560.76847421290518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="8">
-        <v>20</v>
-      </c>
-      <c r="C11" s="8">
-        <v>6</v>
-      </c>
-      <c r="D11" s="8">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>14</v>
-      </c>
-      <c r="E11" s="8">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>30</v>
-      </c>
-      <c r="F11" s="8">
-        <v>341.18200000000002</v>
-      </c>
-      <c r="G11" s="9">
-        <v>192826</v>
-      </c>
-      <c r="H11" s="8">
-        <v>14085</v>
-      </c>
-      <c r="I11" s="8">
-        <v>-155.63</v>
-      </c>
-      <c r="J11">
-        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>13929.37</v>
-      </c>
-      <c r="K11">
-        <f>_xlfn.RANK.EQ(J11, $J$2:$J$15, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="L11" s="16">
-        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13905.603668851065</v>
-      </c>
-      <c r="M11">
-        <v>50000</v>
-      </c>
-      <c r="N11">
-        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4643</v>
-      </c>
-      <c r="O11">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>565.17049551265893</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>13</v>
-      </c>
-      <c r="E12" s="1">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>35</v>
-      </c>
-      <c r="F12" s="1">
-        <v>364.02600000000001</v>
-      </c>
-      <c r="G12" s="3">
-        <v>207507</v>
-      </c>
-      <c r="H12" s="1">
-        <v>14085</v>
-      </c>
-      <c r="I12" s="1">
-        <v>-155.63</v>
-      </c>
-      <c r="J12">
-        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>13929.37</v>
-      </c>
-      <c r="K12">
-        <f>_xlfn.RANK.EQ(J12, $J$2:$J$15, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="L12" s="16">
-        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13929.37</v>
-      </c>
-      <c r="M12">
-        <v>2640000</v>
-      </c>
-      <c r="N12">
-        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4643</v>
-      </c>
-      <c r="O12">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>570.0334591485223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
-        <v>25</v>
-      </c>
-      <c r="F13">
-        <v>369.541</v>
-      </c>
-      <c r="G13" s="12">
-        <v>210117</v>
-      </c>
-      <c r="H13">
-        <v>14085</v>
-      </c>
-      <c r="I13">
-        <v>-226.07</v>
-      </c>
-      <c r="J13">
-        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
-        <v>13858.93</v>
-      </c>
-      <c r="K13">
-        <f>_xlfn.RANK.EQ(J13, $J$2:$J$15, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="L13" s="16">
-        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
-        <v>13851.907010531004</v>
-      </c>
-      <c r="M13">
-        <v>600000</v>
-      </c>
-      <c r="N13">
-        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
-        <v>4635</v>
-      </c>
-      <c r="O13">
-        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
-        <v>568.58914166493025</v>
+        <v>560.13415652786966</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="17">
+        <v>20</v>
+      </c>
+      <c r="C15" s="17">
+        <v>12</v>
+      </c>
+      <c r="D15" s="18">
+        <f>表1[[#This Row],[Games]]-表1[[#This Row],[Wins]]</f>
+        <v>8</v>
+      </c>
+      <c r="E15" s="18">
+        <f>表1[[#This Row],[Wins]]/表1[[#This Row],[Games]]*100</f>
+        <v>60</v>
+      </c>
+      <c r="F15" s="17">
+        <v>396.94200000000001</v>
+      </c>
+      <c r="G15" s="20">
+        <v>218677</v>
+      </c>
+      <c r="H15" s="17">
+        <v>14085</v>
+      </c>
+      <c r="I15" s="17">
+        <v>85.19</v>
+      </c>
+      <c r="J15" s="21">
+        <f>表1[[#This Row],[Baseline ELO]] + 表1[[#This Row],[ELO Difference]]</f>
+        <v>14170.19</v>
+      </c>
+      <c r="K15" s="18">
+        <f>_xlfn.RANK.EQ(J15, $J$2:$J$15, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="L15" s="19">
+        <f>表1[[#This Row],[Calculated Elo]] * (0.8 + 0.2 * (表1[[#This Row],[Efficiency]] / MAX(表1[Efficiency])))</f>
+        <v>14075.084785994464</v>
+      </c>
+      <c r="M15" s="18">
+        <v>3697824</v>
+      </c>
+      <c r="N15" s="18">
+        <f>ROUND( 3000 + 500 *LOG10(表1[[#This Row],[Calculated Elo]] - 11999), 0 )</f>
+        <v>4668</v>
+      </c>
+      <c r="O15" s="18">
+        <f>表1[[#This Row],[Total Playouts]]/表1[[#This Row],[Avg Time (s)]]</f>
+        <v>550.90416232094356</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>